<commit_message>
admin login draft & data base simplification
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Properties</t>
   </si>
@@ -36,36 +36,12 @@
     <t>PropertiesID</t>
   </si>
   <si>
-    <t>PictureId</t>
-  </si>
-  <si>
-    <t>PropertyId</t>
-  </si>
-  <si>
-    <t>PropertyPictures</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
-    <t>FK</t>
-  </si>
-  <si>
     <t>Street</t>
   </si>
   <si>
-    <t>CityId</t>
-  </si>
-  <si>
-    <t>CityName</t>
-  </si>
-  <si>
-    <t>HouseType</t>
-  </si>
-  <si>
-    <t>TypeId</t>
-  </si>
-  <si>
     <t>Area (SQ)</t>
   </si>
   <si>
@@ -90,10 +66,82 @@
     <t>varchar</t>
   </si>
   <si>
-    <t>ImagePath</t>
-  </si>
-  <si>
-    <t>Sale</t>
+    <t>User</t>
+  </si>
+  <si>
+    <t>pswd</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>ImagePath1</t>
+  </si>
+  <si>
+    <t>ImagePath2</t>
+  </si>
+  <si>
+    <t>ImagePath3</t>
+  </si>
+  <si>
+    <t>ImagePath4</t>
+  </si>
+  <si>
+    <t>ImagePath5</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>Burnaby</t>
+  </si>
+  <si>
+    <t>West Vancouver</t>
+  </si>
+  <si>
+    <t>Vancouver West</t>
+  </si>
+  <si>
+    <t>New Westminster</t>
+  </si>
+  <si>
+    <t>Surrey</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>Condo</t>
+  </si>
+  <si>
+    <t>Townhouse</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Duplex</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>(admin)</t>
   </si>
 </sst>
 </file>
@@ -125,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,13 +188,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,7 +207,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -178,14 +220,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,203 +570,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L16"/>
+  <dimension ref="A3:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="8" max="9" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="31.5">
-      <c r="B3" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1">
+    <row r="3" spans="1:9" ht="31.5">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="F5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="C9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="B12" t="s">
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="B13" t="s">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="B14" t="s">
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="B15" t="s">
+      <c r="C25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" t="s">
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
-        <v>23</v>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the plan for the HR Team table
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>Properties</t>
   </si>
@@ -145,13 +145,43 @@
   </si>
   <si>
     <t>News</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Agent Name</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Office Address</t>
+  </si>
+  <si>
+    <t>Office Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Short Bio</t>
+  </si>
+  <si>
+    <t>TEAM TABLE (HR)</t>
+  </si>
+  <si>
+    <t>*is there a phone data type?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,8 +205,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +233,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -210,7 +254,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -235,9 +279,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -253,7 +300,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -295,7 +342,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,27 +374,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,24 +408,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,7 +595,7 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="5" max="6" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,6 +732,10 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
+      <c r="H14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" t="s">
@@ -729,6 +744,12 @@
       <c r="C15" t="s">
         <v>15</v>
       </c>
+      <c r="H15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="B16" t="s">
@@ -737,40 +758,73 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="B17" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="B18" t="s">
         <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="B20" t="s">
         <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -778,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:10">
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
@@ -790,7 +844,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -804,7 +858,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:10">
       <c r="B27" t="s">
         <v>17</v>
       </c>
@@ -815,7 +869,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:10">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -826,7 +880,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:10">
       <c r="E29" t="s">
         <v>40</v>
       </c>
@@ -835,6 +889,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H14:I14"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -842,7 +899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -856,7 +913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated table again with more accurate values.
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Properties</t>
   </si>
@@ -174,7 +174,10 @@
     <t>TEAM TABLE (HR)</t>
   </si>
   <si>
-    <t>*is there a phone data type?</t>
+    <t>Agent ID</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +242,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -254,7 +263,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -281,6 +290,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:J29"/>
+  <dimension ref="A3:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -758,14 +770,14 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="H16" t="s">
-        <v>45</v>
+      <c r="H16" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -773,13 +785,13 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>20</v>
       </c>
@@ -787,16 +799,13 @@
         <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -804,13 +813,13 @@
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:9">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -818,21 +827,27 @@
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:9">
       <c r="B21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
@@ -844,7 +859,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -858,7 +873,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:9">
       <c r="B27" t="s">
         <v>17</v>
       </c>
@@ -869,7 +884,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -880,7 +895,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:9">
       <c r="E29" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
I've added my Sales section. I didn't remove or replace Alan's section just in case there are some questions compared to mine. And I have updated everyone DataType to match with sql commands. There are some tables Alan created previously with can be removed, I just left it there just in case.
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="11865"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>Properties</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Agent Name</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>Office Address</t>
   </si>
   <si>
@@ -178,12 +175,75 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>CityID</t>
+  </si>
+  <si>
+    <t>typeID</t>
+  </si>
+  <si>
+    <t>AUTO_INCREMENT</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>propertyID</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>tinyInt</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Shaun's proposed Sales page &amp; this can be use for SEARCH page too</t>
+  </si>
+  <si>
+    <t>propertyNum</t>
+  </si>
+  <si>
+    <t>streetNum</t>
+  </si>
+  <si>
+    <t>streetName</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>varChar</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>hrID</t>
+  </si>
+  <si>
+    <t>departID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -217,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +308,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -263,7 +329,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -288,11 +354,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -386,6 +455,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -420,6 +490,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -595,317 +666,439 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:I29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="31.5">
-      <c r="B3" s="4"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1">
-      <c r="B5" s="3" t="s">
+    <row r="3" spans="1:12" ht="31.5">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="2" customFormat="1">
+      <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:12">
+      <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
+      <c r="K8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="9" spans="1:12">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="H10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="K15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12">
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12">
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="L18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12">
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="K19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12">
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="K20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12">
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" t="s">
         <v>52</v>
       </c>
-      <c r="I16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="22" spans="4:12">
+      <c r="K22" t="s">
+        <v>48</v>
+      </c>
+      <c r="L22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12">
+      <c r="K23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12">
+      <c r="E25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="4:12">
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12">
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
         <v>15</v>
       </c>
-      <c r="H17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12">
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" t="s">
         <v>15</v>
       </c>
-      <c r="H18" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12">
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
         <v>15</v>
       </c>
-      <c r="H19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="B25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="H29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="E29" t="s">
+    <row r="30" spans="4:12">
+      <c r="H30" t="s">
         <v>40</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I30" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K15:L15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -914,7 +1107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -928,7 +1121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
I have made the Sales editable.html and php. Currently testing it, but it's not working. Will fix it later. The function of the html is, the inputs from user will be immediately displayed below of the html (*this is testing to see whether it works or not).
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>Properties</t>
   </si>
@@ -201,9 +201,6 @@
     <t>city</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>tinyInt</t>
   </si>
   <si>
@@ -213,15 +210,6 @@
     <t>Shaun's proposed Sales page &amp; this can be use for SEARCH page too</t>
   </si>
   <si>
-    <t>propertyNum</t>
-  </si>
-  <si>
-    <t>streetNum</t>
-  </si>
-  <si>
-    <t>streetName</t>
-  </si>
-  <si>
     <t>postalCode</t>
   </si>
   <si>
@@ -231,13 +219,16 @@
     <t>price</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>hrID</t>
   </si>
   <si>
     <t>departID</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>sqFt</t>
   </si>
 </sst>
 </file>
@@ -357,11 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,7 +661,7 @@
   <dimension ref="A3:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,14 +680,14 @@
     </row>
     <row r="4" spans="1:12">
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -750,10 +741,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -770,10 +761,10 @@
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -790,10 +781,10 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>53</v>
@@ -813,10 +804,10 @@
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -833,10 +824,10 @@
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>53</v>
@@ -856,10 +847,10 @@
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -873,10 +864,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -890,10 +881,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -903,30 +894,18 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L15" s="9"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
@@ -948,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="K17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L17" t="s">
         <v>56</v>
@@ -979,7 +958,7 @@
         <v>45</v>
       </c>
       <c r="L19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="4:12">
@@ -1049,7 +1028,7 @@
         <v>56</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I26" t="s">
         <v>56</v>

</xml_diff>